<commit_message>
update code for germany
</commit_message>
<xml_diff>
--- a/data/Germany.xlsx
+++ b/data/Germany.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dangngochuy/Desktop/Hertie/Thesis/Covid19_vs_Climate/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A1237E-F92C-4B48-8826-C8FC7C4DA056}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A55476-F48F-6842-A268-0136F326DE64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{1C915BC3-FB87-6643-8081-B3A8DFCFCE45}"/>
+    <workbookView xWindow="8960" yWindow="1120" windowWidth="27640" windowHeight="16540" xr2:uid="{1C915BC3-FB87-6643-8081-B3A8DFCFCE45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,22 +102,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFD14F69"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF108D90"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF30242D"/>
       <name val="Roboto"/>
     </font>
   </fonts>
@@ -141,14 +125,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -170,13 +152,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>558800</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -231,13 +213,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>31</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>469900</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
+      <xdr:col>41</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -292,13 +274,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>39</xdr:col>
+      <xdr:col>41</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>47</xdr:col>
+      <xdr:col>49</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -353,13 +335,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>47</xdr:col>
+      <xdr:col>49</xdr:col>
       <xdr:colOff>292100</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>55</xdr:col>
+      <xdr:col>57</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -414,13 +396,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>55</xdr:col>
+      <xdr:col>57</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>63</xdr:col>
+      <xdr:col>65</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -475,13 +457,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>63</xdr:col>
+      <xdr:col>65</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>71</xdr:col>
+      <xdr:col>73</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -536,13 +518,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>71</xdr:col>
+      <xdr:col>73</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>78</xdr:col>
+      <xdr:col>80</xdr:col>
       <xdr:colOff>749300</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -597,13 +579,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>78</xdr:col>
+      <xdr:col>80</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>86</xdr:col>
+      <xdr:col>88</xdr:col>
       <xdr:colOff>660400</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -658,13 +640,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>86</xdr:col>
+      <xdr:col>88</xdr:col>
       <xdr:colOff>673100</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>94</xdr:col>
+      <xdr:col>96</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -719,13 +701,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>94</xdr:col>
+      <xdr:col>96</xdr:col>
       <xdr:colOff>584200</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>102</xdr:col>
+      <xdr:col>104</xdr:col>
       <xdr:colOff>482600</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -780,13 +762,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>102</xdr:col>
+      <xdr:col>104</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>110</xdr:col>
+      <xdr:col>112</xdr:col>
       <xdr:colOff>393700</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -841,13 +823,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>110</xdr:col>
+      <xdr:col>112</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>118</xdr:col>
+      <xdr:col>120</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -902,13 +884,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>118</xdr:col>
+      <xdr:col>120</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>126</xdr:col>
+      <xdr:col>128</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -963,13 +945,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>126</xdr:col>
+      <xdr:col>128</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>134</xdr:col>
+      <xdr:col>136</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1024,13 +1006,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>134</xdr:col>
+      <xdr:col>136</xdr:col>
       <xdr:colOff>139700</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>142</xdr:col>
+      <xdr:col>144</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1085,13 +1067,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>142</xdr:col>
+      <xdr:col>144</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>149</xdr:col>
+      <xdr:col>151</xdr:col>
       <xdr:colOff>774700</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1146,13 +1128,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>149</xdr:col>
+      <xdr:col>151</xdr:col>
       <xdr:colOff>787400</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>157</xdr:col>
+      <xdr:col>159</xdr:col>
       <xdr:colOff>685800</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1207,13 +1189,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>157</xdr:col>
+      <xdr:col>159</xdr:col>
       <xdr:colOff>698500</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>165</xdr:col>
+      <xdr:col>167</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1566,318 +1548,433 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A9897A-A686-2B4F-9713-221AE2B405F1}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1" s="2">
+        <v>43906</v>
+      </c>
+      <c r="C1" s="2">
         <v>43905</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2">
+        <v>43893</v>
+      </c>
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
+        <v>2744</v>
+      </c>
+      <c r="C2" s="4">
         <v>2493</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="4">
+        <v>111</v>
+      </c>
+      <c r="E2" s="1">
         <v>7</v>
       </c>
-      <c r="D2" s="4">
+      <c r="F2" s="1">
         <v>15</v>
       </c>
-      <c r="E2" s="1">
+      <c r="G2" s="1">
         <v>66</v>
       </c>
+      <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="1">
+        <v>1105</v>
+      </c>
+      <c r="C3" s="1">
         <v>977</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="1">
+        <v>44</v>
+      </c>
+      <c r="E3" s="1">
         <v>-1</v>
       </c>
-      <c r="D3" s="4">
+      <c r="F3" s="1">
         <v>15</v>
       </c>
-      <c r="E3" s="1">
+      <c r="G3" s="1">
         <v>64</v>
       </c>
+      <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="1">
+        <v>1067</v>
+      </c>
+      <c r="C4" s="1">
         <v>886</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="1">
+        <v>48</v>
+      </c>
+      <c r="E4" s="1">
         <v>-4</v>
       </c>
-      <c r="D4" s="4">
+      <c r="F4" s="1">
         <v>14</v>
       </c>
-      <c r="E4" s="1">
+      <c r="G4" s="1">
         <v>70</v>
       </c>
+      <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="1">
+        <v>391</v>
+      </c>
+      <c r="C5" s="1">
         <v>287</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
         <v>14</v>
       </c>
-      <c r="E5" s="1">
+      <c r="G5" s="1">
         <v>59</v>
       </c>
+      <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="1">
+        <v>342</v>
+      </c>
+      <c r="C6" s="1">
         <v>283</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="1">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="D6" s="4">
+      <c r="F6" s="1">
         <v>12</v>
       </c>
-      <c r="E6" s="1">
+      <c r="G6" s="1">
         <v>46</v>
       </c>
+      <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="1">
+        <v>332</v>
+      </c>
+      <c r="C7" s="1">
         <v>282</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="1">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1">
         <v>3</v>
       </c>
-      <c r="D7" s="4">
+      <c r="F7" s="1">
         <v>14</v>
       </c>
-      <c r="E7" s="1">
+      <c r="G7" s="1">
         <v>62</v>
       </c>
+      <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="1">
+        <v>325</v>
+      </c>
+      <c r="C8" s="1">
         <v>200</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
         <v>3</v>
       </c>
-      <c r="D8" s="4">
+      <c r="F8" s="1">
         <v>14</v>
       </c>
-      <c r="E8" s="1">
+      <c r="G8" s="1">
         <v>62</v>
       </c>
+      <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="1">
+        <v>260</v>
+      </c>
+      <c r="C9" s="1">
         <v>196</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
         <v>3</v>
       </c>
-      <c r="D9" s="4">
+      <c r="F9" s="1">
         <v>14</v>
       </c>
-      <c r="E9" s="1">
+      <c r="G9" s="1">
         <v>61</v>
       </c>
-      <c r="F9">
+      <c r="H9" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="1">
+        <v>152</v>
+      </c>
+      <c r="C10" s="1">
         <v>134</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
         <v>9</v>
       </c>
-      <c r="E10" s="1">
+      <c r="G10" s="1">
         <v>42</v>
       </c>
-      <c r="F10">
+      <c r="H10" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="1">
         <v>123</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1">
+        <v>123</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
         <v>6</v>
       </c>
-      <c r="D11" s="4">
+      <c r="F11" s="1">
         <v>13</v>
       </c>
-      <c r="E11" s="1">
+      <c r="G11" s="1">
         <v>65</v>
       </c>
-      <c r="F11">
+      <c r="H11" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="1">
+        <v>94</v>
+      </c>
+      <c r="C12" s="1">
         <v>84</v>
       </c>
-      <c r="C12" s="3">
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="D12" s="4">
+      <c r="F12" s="1">
         <v>11</v>
       </c>
-      <c r="E12" s="1">
+      <c r="G12" s="1">
         <v>67</v>
       </c>
+      <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="1">
+        <v>85</v>
+      </c>
+      <c r="C13" s="1">
         <v>74</v>
       </c>
-      <c r="C13" s="3">
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
         <v>5</v>
       </c>
-      <c r="D13" s="4">
+      <c r="F13" s="1">
         <v>15</v>
       </c>
-      <c r="E13" s="1">
+      <c r="G13" s="1">
         <v>57</v>
       </c>
-      <c r="F13">
+      <c r="H13" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="1">
+        <v>77</v>
+      </c>
+      <c r="C14" s="1">
         <v>63</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
         <v>3</v>
       </c>
-      <c r="D14" s="4">
+      <c r="F14" s="1">
         <v>12</v>
       </c>
-      <c r="E14" s="1">
+      <c r="G14" s="1">
         <v>54</v>
       </c>
+      <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="1">
+        <v>67</v>
+      </c>
+      <c r="C15" s="1">
         <v>60</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
         <v>7</v>
       </c>
-      <c r="D15" s="4">
+      <c r="F15" s="1">
         <v>14</v>
       </c>
-      <c r="E15" s="1">
+      <c r="G15" s="1">
         <v>45</v>
       </c>
+      <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="1">
+        <v>57</v>
+      </c>
+      <c r="C16" s="1">
         <v>56</v>
       </c>
-      <c r="C16" s="3">
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1">
         <v>5</v>
       </c>
-      <c r="D16" s="4">
+      <c r="F16" s="1">
         <v>14</v>
       </c>
-      <c r="E16" s="1">
+      <c r="G16" s="1">
         <v>68</v>
       </c>
-      <c r="F16">
+      <c r="H16" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="1">
+        <v>51</v>
+      </c>
+      <c r="C17" s="1">
         <v>50</v>
       </c>
-      <c r="C17" s="3">
+      <c r="D17" s="1">
         <v>3</v>
       </c>
-      <c r="D17" s="4">
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1">
         <v>14</v>
       </c>
-      <c r="E17" s="1">
+      <c r="G17" s="1">
         <v>55</v>
       </c>
-      <c r="F17">
+      <c r="H17" s="3">
         <v>19</v>
       </c>
     </row>

</xml_diff>